<commit_message>
Fixed the text not found error.
</commit_message>
<xml_diff>
--- a/src/output/product_data_results.xlsx
+++ b/src/output/product_data_results.xlsx
@@ -468,281 +468,155 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>001.25.791</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>22</v>
-      </c>
+          <t>900.70.061</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>stokta mevcut</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>1.070,54 TL</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>713,69 TL</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>999,17 TL</t>
-        </is>
-      </c>
+          <t>Error</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>001.25.792</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>83</v>
-      </c>
+          <t>900.70.063</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>stokta mevcut</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>1.284,82 TL</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>856,55 TL</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>1.199,17 TL</t>
-        </is>
-      </c>
+          <t>Error</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>001.25.870</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>86</v>
-      </c>
+          <t>900.70.062</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>stokta mevcut</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>2.115,18 TL</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>1.410,12 TL</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>1.974,17 TL</t>
-        </is>
-      </c>
+          <t>Error</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>001.27.205</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>4</v>
-      </c>
+          <t>900.70.066</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
-          <t>stokta mevcut</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>13.026,79 TL</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>8.684,52 TL</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>12.158,33 TL</t>
-        </is>
-      </c>
+          <t>Error</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>001.27.220</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>1</v>
-      </c>
+          <t>900.70.068</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
-          <t>stokta mevcut</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>15.973,21 TL</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>10.648,81 TL</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>14.908,33 TL</t>
-        </is>
-      </c>
+          <t>Error</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>001.27.240</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>2</v>
-      </c>
+          <t>900.70.382</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>stokta mevcut</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>11.241,07 TL</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>7.494,05 TL</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>10.491,67 TL</t>
-        </is>
-      </c>
+          <t>Error</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>001.27.241</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>75</v>
-      </c>
+          <t>900.70.383</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr">
         <is>
-          <t>stokta mevcut</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>5.711,87 TL</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>3.807,92 TL</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>5.331,08 TL</t>
-        </is>
-      </c>
+          <t>Error</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>001.27.250</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>7</v>
-      </c>
+          <t>900.70.384</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr">
         <is>
-          <t>stokta mevcut</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>33.741,07 TL</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>22.494,05 TL</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>31.491,67 TL</t>
-        </is>
-      </c>
+          <t>Error</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>001.25.840</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>4</v>
-      </c>
+          <t>900.70.386</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr">
         <is>
-          <t>stokta mevcut</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>14.544,64 TL</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>9.696,43 TL</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>13.575,00 TL</t>
-        </is>
-      </c>
+          <t>Error</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>001.27.251</t>
+          <t>900.70.388</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -751,17 +625,17 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>10.794,64 TL</t>
+          <t>1.056,73 TL</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>7.196,43 TL</t>
+          <t>704,49 TL</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>10.075,00 TL</t>
+          <t>915,83 TL</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
remove the unnecessary firefox image, fixed the group product error
</commit_message>
<xml_diff>
--- a/src/output/product_data_results.xlsx
+++ b/src/output/product_data_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,174 +468,94 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>900.70.061</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr"/>
+          <t>900.70.391</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>urun hafele.com.tr de bulunmuyor</t>
+        </is>
+      </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Error</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
+          <t>urun hafele.com.tr de bulunmuyor</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>urun hafele.com.tr de bulunmuyor</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>urun hafele.com.tr de bulunmuyor</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>urun hafele.com.tr de bulunmuyor</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>900.70.063</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr"/>
+          <t>900.78.217</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>urun hafele.com.tr de bulunmuyor</t>
+        </is>
+      </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Error</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
+          <t>urun hafele.com.tr de bulunmuyor</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>urun hafele.com.tr de bulunmuyor</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>urun hafele.com.tr de bulunmuyor</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>urun hafele.com.tr de bulunmuyor</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>900.70.062</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr"/>
+          <t>900.78.417</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1238</v>
+      </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Error</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>900.70.066</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Error</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>900.70.068</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Error</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>900.70.382</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Error</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>900.70.383</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Error</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>900.70.384</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Error</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>900.70.386</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Error</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>900.70.388</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>7</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>stokta mevcut</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>1.056,73 TL</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>704,49 TL</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>915,83 TL</t>
+          <t>set urun</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2.040,34 TL</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>1.360,22 TL</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>1.768,29 TL</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Commit message for your changes
</commit_message>
<xml_diff>
--- a/src/output/product_data_results.xlsx
+++ b/src/output/product_data_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,94 +468,426 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>900.70.391</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>urun hafele.com.tr de bulunmuyor</t>
-        </is>
+          <t>903.52.718</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>42</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>urun hafele.com.tr de bulunmuyor</t>
+          <t>stokta mevcut</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>urun hafele.com.tr de bulunmuyor</t>
+          <t>315,34 TL</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>urun hafele.com.tr de bulunmuyor</t>
+          <t>210,22 TL</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>urun hafele.com.tr de bulunmuyor</t>
+          <t>273,29 TL</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>900.78.217</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>urun hafele.com.tr de bulunmuyor</t>
-        </is>
+          <t>903.53.718</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>21</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>urun hafele.com.tr de bulunmuyor</t>
+          <t>stokta mevcut</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>urun hafele.com.tr de bulunmuyor</t>
+          <t>657,64 TL</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>urun hafele.com.tr de bulunmuyor</t>
+          <t>438,43 TL</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>urun hafele.com.tr de bulunmuyor</t>
+          <t>569,96 TL</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>900.78.417</t>
+          <t>903.58.055</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1238</v>
+        <v>87</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>set urun</t>
+          <t>stokta mevcut</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2.040,34 TL</t>
+          <t>136,49 TL</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.360,22 TL</t>
+          <t>90,99 TL</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>1.768,29 TL</t>
+          <t>118,29 TL</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>903.58.056</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>55</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>stokta mevcut</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>136,49 TL</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>90,99 TL</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>118,29 TL</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>903.58.064</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>urun hafele.com.tr de bulunmuyor</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>urun hafele.com.tr de bulunmuyor</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>urun hafele.com.tr de bulunmuyor</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>urun hafele.com.tr de bulunmuyor</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>urun hafele.com.tr de bulunmuyor</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>903.58.057</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>66</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>stokta mevcut</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>383,61 TL</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>255,74 TL</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>332,46 TL</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>903.58.068</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>93</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>stokta mevcut</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>148,03 TL</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>98,69 TL</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>128,29 TL</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>903.58.070</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>urun hafele.com.tr de bulunmuyor</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>urun hafele.com.tr de bulunmuyor</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>urun hafele.com.tr de bulunmuyor</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>urun hafele.com.tr de bulunmuyor</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>urun hafele.com.tr de bulunmuyor</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>903.58.067</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>847</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>stokta mevcut</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>114,38 TL</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>76,25 TL</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>99,13 TL</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>903.58.114</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>urun hafele.com.tr de bulunmuyor</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>urun hafele.com.tr de bulunmuyor</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>urun hafele.com.tr de bulunmuyor</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>urun hafele.com.tr de bulunmuyor</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>urun hafele.com.tr de bulunmuyor</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>903.58.267</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>stokta mevcut</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>72,06 TL</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>48,04 TL</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>62,46 TL</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>903.58.323</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>806</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>stokta mevcut</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>157,64 TL</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>105,10 TL</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>136,63 TL</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>903.58.368</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>143</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>stokta mevcut</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>99,95 TL</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>66,63 TL</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>86,63 TL</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>903.70.124</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>3 ila 5 gün içinde</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>614,24 TL</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>409,49 TL</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>573,29 TL</t>
         </is>
       </c>
     </row>

</xml_diff>